<commit_message>
Advancing run off of new plants
</commit_message>
<xml_diff>
--- a/hydropower_list_seasonal.xlsx
+++ b/hydropower_list_seasonal.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>capacity</t>
+          <t>Total capacity (MW)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -2090,7 +2090,7 @@
         <v>66</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="I38" t="n">
         <v>263.11</v>
@@ -2134,7 +2134,7 @@
         <v>104</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="I39" t="n">
         <v>448.2</v>
@@ -2784,7 +2784,7 @@
         <v>260</v>
       </c>
       <c r="H54" t="n">
-        <v>65</v>
+        <v>260</v>
       </c>
       <c r="I54" t="n">
         <v>2009</v>
@@ -3130,7 +3130,7 @@
         <v>54</v>
       </c>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I62" t="n">
         <v>198.2</v>
@@ -3174,7 +3174,7 @@
         <v>160</v>
       </c>
       <c r="H63" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I63" t="n">
         <v>633</v>
@@ -3387,7 +3387,7 @@
         <v>102.5477160000035</v>
       </c>
       <c r="G68" t="n">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H68" t="n">
         <v>40</v>

</xml_diff>